<commit_message>
Update for readme file
</commit_message>
<xml_diff>
--- a/Manual_vs_Automation_comparision.xlsx
+++ b/Manual_vs_Automation_comparision.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shivanand\BITS_WILP\4thsem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f002f89e365d7a/Documents/GitHub/pythonsel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CFECE7-C1FE-4FCA-86F4-7CB3CF05A5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{99CFECE7-C1FE-4FCA-86F4-7CB3CF05A5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8944011E-1022-4C45-84CE-35F3A6E9B0D6}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" xr2:uid="{0C9EAFDC-EC0B-4984-8E36-6CB05F3ACB30}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -40,11 +40,6 @@
   </si>
   <si>
     <t>Expected Result</t>
-  </si>
-  <si>
-    <t>1) Open Google Chrome
-2) Launch the Orange HRM web URL
-3) Login using valid credentials</t>
   </si>
   <si>
     <t xml:space="preserve">Launch Orange HRM </t>
@@ -178,23 +173,45 @@
     <t>Automation time to execute</t>
   </si>
   <si>
-    <t>1 min</t>
-  </si>
-  <si>
-    <t>0.5 sec</t>
-  </si>
-  <si>
-    <t>3 min</t>
-  </si>
-  <si>
-    <t>0.2 sec</t>
-  </si>
-  <si>
-    <t>0.3 sec</t>
-  </si>
-  <si>
     <t>Orange HRM
 Release 1.0 - Funtional Test - Approximate Estimation Manual vs Automation time taken/effort</t>
+  </si>
+  <si>
+    <t>3 sec</t>
+  </si>
+  <si>
+    <t>4 sec</t>
+  </si>
+  <si>
+    <t>5 sec</t>
+  </si>
+  <si>
+    <t>2 sec</t>
+  </si>
+  <si>
+    <t>2 min</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>29 sec</t>
+  </si>
+  <si>
+    <t>1) Open Google Chrome
+2) Launch the Orange HRM web URL</t>
+  </si>
+  <si>
+    <t>8 sec</t>
+  </si>
+  <si>
+    <t>6 sec</t>
+  </si>
+  <si>
+    <t>Total time execution</t>
+  </si>
+  <si>
+    <t>59 sec</t>
   </si>
 </sst>
 </file>
@@ -265,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -290,6 +307,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29AF77B-D836-4648-801E-54FC5CDEA9F7}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -623,7 +646,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -650,30 +673,30 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>47</v>
@@ -681,163 +704,174 @@
     </row>
     <row r="6" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>